<commit_message>
DB login and Login func fixed
</commit_message>
<xml_diff>
--- a/src/test/java/_02_ApachePOI/Resources/ApacheExcel22.xlsx
+++ b/src/test/java/_02_ApachePOI/Resources/ApacheExcel22.xlsx
@@ -5,29 +5,28 @@
   <fileSharing readOnlyRecommended="0" userName="yyoldas" reservationPassword="ED25"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="4" xWindow="240" yWindow="60" windowWidth="17280" windowHeight="8970" tabRatio="500"/>
+    <workbookView activeTab="3" xWindow="240" yWindow="60" windowWidth="17280" windowHeight="8970" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet name="testCitizen" sheetId="2" r:id="rId5"/>
     <sheet name="AddNewAddress" sheetId="3" r:id="rId6"/>
     <sheet name="Nation" sheetId="4" r:id="rId7"/>
-    <sheet name="Login" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1668205125" val="1054" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1668205125" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1668205125" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1668205125"/>
+      <pm:revision xmlns:pm="smNativeData" day="1668522235" val="1054" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1668522235" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1668522235" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1668522235"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
   <si>
     <t>Lion</t>
   </si>
@@ -96,12 +95,6 @@
   </si>
   <si>
     <t>USAINDIA2</t>
-  </si>
-  <si>
-    <t>richfield.edu</t>
-  </si>
-  <si>
-    <t>Richfield2020!</t>
   </si>
 </sst>
 </file>
@@ -127,7 +120,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1668205125" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1668522235" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -142,7 +135,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1668205125" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1668522235" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -175,7 +168,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1668205125"/>
+          <pm:border xmlns:pm="smNativeData" id="1668522235"/>
         </ext>
       </extLst>
     </border>
@@ -196,10 +189,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1668205125" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1668522235" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1668205125" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1668522235" count="2">
         <pm:color name="Color 26" rgb="9876AA"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
       </pm:colors>
@@ -543,7 +536,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1668205125" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1668522235" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -552,16 +545,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1668522235" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1668522235" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1668522235" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1668522235" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1668205125" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1668522235" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -753,7 +746,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1668205125" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1668522235" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -762,16 +755,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1668522235" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1668522235" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1668522235" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1668522235" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1668205125" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1668522235" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -860,7 +853,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1668205125" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1668522235" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -869,16 +862,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1668522235" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1668522235" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1668522235" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1668522235" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1668205125" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1668522235" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -891,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -921,7 +914,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1668205125" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1668522235" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -930,68 +923,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1668522235" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1668522235" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1668522235" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1668522235" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1668205125" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="15.40"/>
-  <cols>
-    <col min="1" max="2" width="12.312500" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1668205125" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
-  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1668205125" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1668205125" Id="1" type="0" value="0"/>
-      </ext>
-    </extLst>
-  </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1668205125" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1668522235" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>